<commit_message>
Added 3D model, Gerbers, Layout, Project files, and updated BOM and Schematic
</commit_message>
<xml_diff>
--- a/BOM/DVM_BOM.xlsx
+++ b/BOM/DVM_BOM.xlsx
@@ -1,718 +1,751 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Desktop\OrCAD Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERS\LUCY\DESKTOP\ORCAD PRACTICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4D8FBFCC-91EB-495F-BCC0-220391BB6C0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{556E2934-D883-4760-B2D6-9A12AD3212C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="1875" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="5250" yWindow="3075" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="DVM" sheetId="1" r:id="rId1"/>
+    <sheet name="DVM_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="242">
+  <si>
+    <t>DVM - Cover  Revised: Thursday, April 18, 2019</t>
+  </si>
   <si>
     <t>01          Revision: A</t>
   </si>
   <si>
+    <t>Bill Of Materials          April 18,2019      12:12:42</t>
+  </si>
+  <si>
+    <t>Page1</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Manufacturer_Part_Number</t>
+  </si>
+  <si>
+    <t>______________________________________________</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>TMK107BBJ106MA-T</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>0.47uF</t>
+  </si>
+  <si>
+    <t>TMK107B7474KA-TR</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>TMK107B7105KA-T</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R7BB104</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C0805X475J9RAC7800</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>0.22uF</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R6BB224</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>510p</t>
+  </si>
+  <si>
+    <t>CC0603JRNPO9BN511</t>
+  </si>
+  <si>
+    <t>DS1</t>
+  </si>
+  <si>
+    <t>LDF-A5616RI</t>
+  </si>
+  <si>
+    <t>Lumex</t>
+  </si>
+  <si>
+    <t>DS2</t>
+  </si>
+  <si>
+    <t>LDS-SMHTA304RISITR</t>
+  </si>
+  <si>
+    <t>Lumex Opto/Components Inc.</t>
+  </si>
+  <si>
+    <t>DS3</t>
+  </si>
+  <si>
+    <t>DS4</t>
+  </si>
+  <si>
+    <t>DS5</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>1N914BWS</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t>SML-D12U1WT86</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>HEADER 1</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>TSW-101-07-F-S</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>575-4</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>HEADER 2</t>
+  </si>
+  <si>
+    <t>TSW-102-07-F-S</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>MTG1</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>MTG2</t>
+  </si>
+  <si>
+    <t>MTG3</t>
+  </si>
+  <si>
+    <t>MTG4</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>NPN BCE</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>DNBT8105-7</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>PNP BCE</t>
+  </si>
+  <si>
+    <t>DPBT8105-7</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RC0603JR-0710KL</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RT0603BRD07390RL</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>1.8M</t>
+  </si>
+  <si>
+    <t>RC0603FR-071M8L</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>180k</t>
+  </si>
+  <si>
+    <t>RT0603BRD07180KL</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>18k</t>
+  </si>
+  <si>
+    <t>RT0603BRD0718KL</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>RT0603BRD072KL</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>2.49k</t>
+  </si>
+  <si>
+    <t>RC0603FR-072K49L</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K5L</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>RC0603FR-07150RL</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0727KL</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>6.8k</t>
+  </si>
+  <si>
+    <t>RC0603FR-076K8L</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>16k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0716KL</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>56k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0756KL</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0730KL</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>RC0603FR-07140RL</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>RC0603FR-0739KL</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>RC0603JR-070RL</t>
+  </si>
+  <si>
+    <t>R54</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>TP1</t>
+  </si>
+  <si>
+    <t>5V+</t>
+  </si>
+  <si>
+    <t>TP2</t>
+  </si>
+  <si>
+    <t>Power_In</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>5V-</t>
+  </si>
+  <si>
+    <t>TP4</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>TP5</t>
+  </si>
+  <si>
+    <t>V_REF_1V2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>TLC7135</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TLC7135CDWR</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TLP175A</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>TLP175A(TPL,E</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SN74LVC1G32DBVR</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>SN7447</t>
+  </si>
+  <si>
+    <t>SN7447AN</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>NCP1117ST50T3G</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>MAX1044CSA</t>
+  </si>
+  <si>
+    <t>Maxim Integrated</t>
+  </si>
+  <si>
+    <t>MAX1044CSA+</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>MAX8069ESA+</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>LM311</t>
+  </si>
+  <si>
+    <t>LM311DR</t>
+  </si>
+  <si>
     <t>Nosherwan Ahmed</t>
-  </si>
-  <si>
-    <t>Bill Of Materials          March 11,2019      17:14:07</t>
-  </si>
-  <si>
-    <t>Page1</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Part</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Manufacturer_Part_Number</t>
-  </si>
-  <si>
-    <t>______________________________________________</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>Taiyo Yuden</t>
-  </si>
-  <si>
-    <t>TMK107BBJ106MA-T</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C16</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>0.47uF</t>
-  </si>
-  <si>
-    <t>TMK107B7474KA-TR</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>TMK107B7105KA-T</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>CC0603JRX7R7BB104</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>C0805X475J9RAC7800</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>0.22uF</t>
-  </si>
-  <si>
-    <t>CC0603JRX7R6BB224</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>510p</t>
-  </si>
-  <si>
-    <t>CC0603JRNPO9BN511</t>
-  </si>
-  <si>
-    <t>DS1</t>
-  </si>
-  <si>
-    <t>LDF-A5616RI</t>
-  </si>
-  <si>
-    <t>Lumex</t>
-  </si>
-  <si>
-    <t>DS2</t>
-  </si>
-  <si>
-    <t>LDS-SMHTA304RISITR</t>
-  </si>
-  <si>
-    <t>Lumex Opto/Components Inc.</t>
-  </si>
-  <si>
-    <t>DS3</t>
-  </si>
-  <si>
-    <t>DS4</t>
-  </si>
-  <si>
-    <t>DS5</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>DIODE</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>1N914BWS</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
-    <t>SML-D12U1WT86</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>HEADER 1</t>
-  </si>
-  <si>
-    <t>Samtec Inc.</t>
-  </si>
-  <si>
-    <t>TSW-101-07-F-S</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>575-4</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>HEADER 2</t>
-  </si>
-  <si>
-    <t>TSW-102-07-F-S</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>NPN BCE</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>DNBT8105-7</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>Q8</t>
-  </si>
-  <si>
-    <t>Q10</t>
-  </si>
-  <si>
-    <t>Q11</t>
-  </si>
-  <si>
-    <t>Q12</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
-    <t>PNP BCE</t>
-  </si>
-  <si>
-    <t>DPBT8105-7</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RC0603JR-0710KL</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>RC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>RT0603BRD07390RL</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>1.8M</t>
-  </si>
-  <si>
-    <t>RC0603FR-071M8L</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>180k</t>
-  </si>
-  <si>
-    <t>RT0603BRD07180KL</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>RT0603BRD0718KL</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>2k</t>
-  </si>
-  <si>
-    <t>RT0603BRD072KL</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>2.49k</t>
-  </si>
-  <si>
-    <t>RC0603FR-072K49L</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>1.5k</t>
-  </si>
-  <si>
-    <t>RC0603FR-071K5L</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>RC0603FR-07150RL</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>47k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>RC0603FR-074K7L</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>27k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0727KL</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>6.8k</t>
-  </si>
-  <si>
-    <t>RC0603FR-076K8L</t>
-  </si>
-  <si>
-    <t>R41</t>
-  </si>
-  <si>
-    <t>16k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0716KL</t>
-  </si>
-  <si>
-    <t>R45</t>
-  </si>
-  <si>
-    <t>R42</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>RC0603FR-071KL</t>
-  </si>
-  <si>
-    <t>R43</t>
-  </si>
-  <si>
-    <t>56k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0756KL</t>
-  </si>
-  <si>
-    <t>R44</t>
-  </si>
-  <si>
-    <t>30k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0730KL</t>
-  </si>
-  <si>
-    <t>R46</t>
-  </si>
-  <si>
-    <t>RC0603FR-07140RL</t>
-  </si>
-  <si>
-    <t>R47</t>
-  </si>
-  <si>
-    <t>R48</t>
-  </si>
-  <si>
-    <t>R49</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t>R51</t>
-  </si>
-  <si>
-    <t>R52</t>
-  </si>
-  <si>
-    <t>39k</t>
-  </si>
-  <si>
-    <t>RC0603FR-0739KL</t>
-  </si>
-  <si>
-    <t>TP1</t>
-  </si>
-  <si>
-    <t>5V+</t>
-  </si>
-  <si>
-    <t>TP2</t>
-  </si>
-  <si>
-    <t>Power_In</t>
-  </si>
-  <si>
-    <t>TP3</t>
-  </si>
-  <si>
-    <t>5V-</t>
-  </si>
-  <si>
-    <t>TP4</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>TP5</t>
-  </si>
-  <si>
-    <t>V_REF_1V2</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>TLC7135</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>TLC7135CDWR</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TLP175A</t>
-  </si>
-  <si>
-    <t>Toshiba Semiconductor and Storage</t>
-  </si>
-  <si>
-    <t>TLP175A(TPL,E</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>SN74LVC1G32DBVR</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>SN7447</t>
-  </si>
-  <si>
-    <t>SN7447AN</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>NCP1117ST50T3G</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>MAX1044CSA</t>
-  </si>
-  <si>
-    <t>Maxim Integrated</t>
-  </si>
-  <si>
-    <t>MAX1044CSA+</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>MAX8069ESA+</t>
-  </si>
-  <si>
-    <t>U11</t>
-  </si>
-  <si>
-    <t>LM311</t>
-  </si>
-  <si>
-    <t>LM311DR</t>
-  </si>
-  <si>
-    <t>DVM Revised: Monday, March 11, 2019</t>
   </si>
 </sst>
 </file>
@@ -1553,13 +1586,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
@@ -1568,17 +1604,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2269,7 +2305,7 @@
         <v>16</v>
       </c>
       <c r="B55">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
         <v>87</v>
@@ -2281,12 +2317,12 @@
         <v>89</v>
       </c>
       <c r="F55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D56" t="s">
         <v>88</v>
@@ -2295,12 +2331,12 @@
         <v>89</v>
       </c>
       <c r="F56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D57" t="s">
         <v>88</v>
@@ -2309,12 +2345,12 @@
         <v>89</v>
       </c>
       <c r="F57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s">
         <v>88</v>
@@ -2323,263 +2359,263 @@
         <v>89</v>
       </c>
       <c r="F58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <v>11</v>
+      </c>
       <c r="C59" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" t="s">
         <v>94</v>
       </c>
-      <c r="D59" t="s">
-        <v>88</v>
-      </c>
       <c r="E59" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F59" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" t="s">
         <v>95</v>
       </c>
-      <c r="D60" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" t="s">
-        <v>89</v>
-      </c>
       <c r="F60" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" t="s">
         <v>96</v>
-      </c>
-      <c r="D61" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" t="s">
-        <v>89</v>
-      </c>
-      <c r="F61" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D62" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E62" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F62" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F63" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D64" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E64" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F64" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F65" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>17</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D66" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E66" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F66" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>18</v>
-      </c>
-      <c r="B67">
-        <v>8</v>
-      </c>
       <c r="C67" t="s">
         <v>104</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E67" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="F67" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E68" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="F68" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" t="s">
         <v>108</v>
       </c>
-      <c r="D69" t="s">
-        <v>105</v>
-      </c>
-      <c r="E69" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+      <c r="E70" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" t="s">
         <v>109</v>
       </c>
-      <c r="D70" t="s">
-        <v>105</v>
-      </c>
-      <c r="E70" t="s">
-        <v>32</v>
-      </c>
-      <c r="F70" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>19</v>
+      </c>
+      <c r="B71">
+        <v>8</v>
+      </c>
       <c r="C71" t="s">
         <v>110</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E71" t="s">
         <v>32</v>
       </c>
       <c r="F71" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
+        <v>113</v>
+      </c>
+      <c r="D72" t="s">
         <v>111</v>
       </c>
-      <c r="D72" t="s">
-        <v>105</v>
-      </c>
       <c r="E72" t="s">
         <v>32</v>
       </c>
       <c r="F72" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" t="s">
+        <v>111</v>
+      </c>
+      <c r="E73" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" t="s">
         <v>112</v>
-      </c>
-      <c r="D73" t="s">
-        <v>105</v>
-      </c>
-      <c r="E73" t="s">
-        <v>32</v>
-      </c>
-      <c r="F73" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D74" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E74" t="s">
         <v>32</v>
       </c>
       <c r="F74" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>19</v>
-      </c>
-      <c r="B75">
-        <v>2</v>
-      </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D75" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E75" t="s">
         <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2587,172 +2623,166 @@
         <v>117</v>
       </c>
       <c r="D76" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E76" t="s">
         <v>32</v>
       </c>
       <c r="F76" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>20</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
       <c r="C77" t="s">
         <v>118</v>
       </c>
-      <c r="D77">
-        <v>390</v>
+      <c r="D77" t="s">
+        <v>111</v>
       </c>
       <c r="E77" t="s">
         <v>32</v>
       </c>
       <c r="F77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>21</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
-        <v>120</v>
-      </c>
       <c r="D78" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E78" t="s">
         <v>32</v>
       </c>
       <c r="F78" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" t="s">
+        <v>121</v>
+      </c>
+      <c r="E79" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>123</v>
       </c>
-      <c r="D79" t="s">
-        <v>124</v>
-      </c>
-      <c r="E79" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>23</v>
-      </c>
-      <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="C80" t="s">
-        <v>126</v>
-      </c>
       <c r="D80" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E80" t="s">
         <v>32</v>
       </c>
       <c r="F80" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>129</v>
-      </c>
-      <c r="D81" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="D81">
+        <v>390</v>
       </c>
       <c r="E81" t="s">
         <v>32</v>
       </c>
       <c r="F81" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D82" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E82" t="s">
         <v>32</v>
       </c>
       <c r="F82" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C83" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" t="s">
+        <v>130</v>
+      </c>
+      <c r="E83" t="s">
+        <v>32</v>
+      </c>
+      <c r="F83" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>24</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>132</v>
+      </c>
+      <c r="D84" t="s">
+        <v>133</v>
+      </c>
+      <c r="E84" t="s">
+        <v>32</v>
+      </c>
+      <c r="F84" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>25</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
         <v>135</v>
-      </c>
-      <c r="D83" t="s">
-        <v>136</v>
-      </c>
-      <c r="E83" t="s">
-        <v>32</v>
-      </c>
-      <c r="F83" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>138</v>
-      </c>
-      <c r="D84" t="s">
-        <v>136</v>
-      </c>
-      <c r="E84" t="s">
-        <v>32</v>
-      </c>
-      <c r="F84" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>139</v>
       </c>
       <c r="D85" t="s">
         <v>136</v>
@@ -2765,17 +2795,23 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>26</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
       <c r="C86" t="s">
+        <v>138</v>
+      </c>
+      <c r="D86" t="s">
+        <v>139</v>
+      </c>
+      <c r="E86" t="s">
+        <v>32</v>
+      </c>
+      <c r="F86" t="s">
         <v>140</v>
-      </c>
-      <c r="D86" t="s">
-        <v>136</v>
-      </c>
-      <c r="E86" t="s">
-        <v>32</v>
-      </c>
-      <c r="F86" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2783,66 +2819,72 @@
         <v>27</v>
       </c>
       <c r="B87">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C87" t="s">
         <v>141</v>
       </c>
-      <c r="D87">
-        <v>150</v>
+      <c r="D87" t="s">
+        <v>142</v>
       </c>
       <c r="E87" t="s">
         <v>32</v>
       </c>
       <c r="F87" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
+        <v>144</v>
+      </c>
+      <c r="D88" t="s">
+        <v>142</v>
+      </c>
+      <c r="E88" t="s">
+        <v>32</v>
+      </c>
+      <c r="F88" t="s">
         <v>143</v>
-      </c>
-      <c r="D88">
-        <v>150</v>
-      </c>
-      <c r="E88" t="s">
-        <v>32</v>
-      </c>
-      <c r="F88" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D89">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="D89" t="s">
+        <v>142</v>
       </c>
       <c r="E89" t="s">
         <v>32</v>
       </c>
       <c r="F89" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>145</v>
-      </c>
-      <c r="D90">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="D90" t="s">
+        <v>142</v>
       </c>
       <c r="E90" t="s">
         <v>32</v>
       </c>
       <c r="F90" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>28</v>
+      </c>
+      <c r="B91">
+        <v>13</v>
+      </c>
       <c r="C91" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D91">
         <v>150</v>
@@ -2851,12 +2893,12 @@
         <v>32</v>
       </c>
       <c r="F91" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D92">
         <v>150</v>
@@ -2865,12 +2907,12 @@
         <v>32</v>
       </c>
       <c r="F92" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D93">
         <v>150</v>
@@ -2879,12 +2921,12 @@
         <v>32</v>
       </c>
       <c r="F93" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D94">
         <v>150</v>
@@ -2893,12 +2935,12 @@
         <v>32</v>
       </c>
       <c r="F94" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D95">
         <v>150</v>
@@ -2907,12 +2949,12 @@
         <v>32</v>
       </c>
       <c r="F95" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D96">
         <v>150</v>
@@ -2921,12 +2963,12 @@
         <v>32</v>
       </c>
       <c r="F96" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D97">
         <v>150</v>
@@ -2935,12 +2977,12 @@
         <v>32</v>
       </c>
       <c r="F97" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D98">
         <v>150</v>
@@ -2949,12 +2991,12 @@
         <v>32</v>
       </c>
       <c r="F98" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D99">
         <v>150</v>
@@ -2963,290 +3005,290 @@
         <v>32</v>
       </c>
       <c r="F99" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>28</v>
-      </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
       <c r="C100" t="s">
-        <v>155</v>
-      </c>
-      <c r="D100" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="D100">
+        <v>150</v>
       </c>
       <c r="E100" t="s">
         <v>32</v>
       </c>
       <c r="F100" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>29</v>
-      </c>
-      <c r="B101">
-        <v>2</v>
-      </c>
       <c r="C101" t="s">
         <v>158</v>
       </c>
-      <c r="D101" t="s">
-        <v>159</v>
+      <c r="D101">
+        <v>150</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
       </c>
       <c r="F101" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
+        <v>159</v>
+      </c>
+      <c r="D102">
+        <v>150</v>
+      </c>
+      <c r="E102" t="s">
+        <v>32</v>
+      </c>
+      <c r="F102" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>160</v>
+      </c>
+      <c r="D103">
+        <v>150</v>
+      </c>
+      <c r="E103" t="s">
+        <v>32</v>
+      </c>
+      <c r="F103" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>29</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
         <v>161</v>
       </c>
-      <c r="D102" t="s">
-        <v>159</v>
-      </c>
-      <c r="E102" t="s">
-        <v>32</v>
-      </c>
-      <c r="F102" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="D104" t="s">
+        <v>162</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
         <v>30</v>
       </c>
-      <c r="B103">
-        <v>3</v>
-      </c>
-      <c r="C103" t="s">
-        <v>162</v>
-      </c>
-      <c r="D103" t="s">
-        <v>163</v>
-      </c>
-      <c r="E103" t="s">
-        <v>32</v>
-      </c>
-      <c r="F103" t="s">
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+      <c r="D105" t="s">
         <v>165</v>
       </c>
-      <c r="D104" t="s">
-        <v>163</v>
-      </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
+      <c r="E105" t="s">
+        <v>32</v>
+      </c>
+      <c r="F105" t="s">
         <v>166</v>
       </c>
-      <c r="D105" t="s">
-        <v>163</v>
-      </c>
-      <c r="E105" t="s">
-        <v>32</v>
-      </c>
-      <c r="F105" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>31</v>
-      </c>
-      <c r="B106">
-        <v>1</v>
-      </c>
       <c r="C106" t="s">
         <v>167</v>
       </c>
       <c r="D106" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
       </c>
       <c r="F106" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" t="s">
+        <v>169</v>
+      </c>
+      <c r="E107" t="s">
+        <v>32</v>
+      </c>
+      <c r="F107" t="s">
         <v>170</v>
-      </c>
-      <c r="D107" t="s">
-        <v>171</v>
-      </c>
-      <c r="E107" t="s">
-        <v>32</v>
-      </c>
-      <c r="F107" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D108" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
       </c>
       <c r="F108" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>33</v>
-      </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-      <c r="C109" t="s">
-        <v>174</v>
-      </c>
       <c r="D109" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E109" t="s">
         <v>32</v>
       </c>
       <c r="F109" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D110" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E110" t="s">
         <v>32</v>
       </c>
       <c r="F110" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
+        <v>33</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>176</v>
+      </c>
+      <c r="D111" t="s">
+        <v>177</v>
+      </c>
+      <c r="E111" t="s">
+        <v>32</v>
+      </c>
+      <c r="F111" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>179</v>
+      </c>
+      <c r="D112" t="s">
+        <v>177</v>
+      </c>
+      <c r="E112" t="s">
+        <v>32</v>
+      </c>
+      <c r="F112" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>34</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>180</v>
+      </c>
+      <c r="D113" t="s">
+        <v>181</v>
+      </c>
+      <c r="E113" t="s">
+        <v>32</v>
+      </c>
+      <c r="F113" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
         <v>35</v>
       </c>
-      <c r="B111">
+      <c r="B114">
         <v>1</v>
       </c>
-      <c r="C111" t="s">
-        <v>180</v>
-      </c>
-      <c r="D111" t="s">
-        <v>181</v>
-      </c>
-      <c r="E111" t="s">
-        <v>32</v>
-      </c>
-      <c r="F111" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112">
+      <c r="C114" t="s">
+        <v>183</v>
+      </c>
+      <c r="D114" t="s">
+        <v>184</v>
+      </c>
+      <c r="E114" t="s">
+        <v>32</v>
+      </c>
+      <c r="F114" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
         <v>36</v>
       </c>
-      <c r="B112">
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s">
+        <v>186</v>
+      </c>
+      <c r="D115" t="s">
+        <v>187</v>
+      </c>
+      <c r="E115" t="s">
+        <v>32</v>
+      </c>
+      <c r="F115" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>37</v>
+      </c>
+      <c r="B116">
         <v>6</v>
       </c>
-      <c r="C112" t="s">
-        <v>183</v>
-      </c>
-      <c r="D112">
-        <v>140</v>
-      </c>
-      <c r="E112" t="s">
-        <v>32</v>
-      </c>
-      <c r="F112" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>185</v>
-      </c>
-      <c r="D113">
-        <v>140</v>
-      </c>
-      <c r="E113" t="s">
-        <v>32</v>
-      </c>
-      <c r="F113" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C114" t="s">
-        <v>186</v>
-      </c>
-      <c r="D114">
-        <v>140</v>
-      </c>
-      <c r="E114" t="s">
-        <v>32</v>
-      </c>
-      <c r="F114" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
-        <v>187</v>
-      </c>
-      <c r="D115">
-        <v>140</v>
-      </c>
-      <c r="E115" t="s">
-        <v>32</v>
-      </c>
-      <c r="F115" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D116">
         <v>140</v>
@@ -3255,12 +3297,12 @@
         <v>32</v>
       </c>
       <c r="F116" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D117">
         <v>140</v>
@@ -3269,329 +3311,447 @@
         <v>32</v>
       </c>
       <c r="F117" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>37</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
       <c r="C118" t="s">
+        <v>192</v>
+      </c>
+      <c r="D118">
+        <v>140</v>
+      </c>
+      <c r="E118" t="s">
+        <v>32</v>
+      </c>
+      <c r="F118" t="s">
         <v>190</v>
       </c>
-      <c r="D118" t="s">
-        <v>191</v>
-      </c>
-      <c r="E118" t="s">
-        <v>32</v>
-      </c>
-      <c r="F118" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>38</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
       <c r="C119" t="s">
         <v>193</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119">
+        <v>140</v>
+      </c>
+      <c r="E119" t="s">
+        <v>32</v>
+      </c>
+      <c r="F119" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
         <v>194</v>
       </c>
-      <c r="E119" t="s">
-        <v>78</v>
-      </c>
-      <c r="F119">
-        <v>5029</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>39</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="D120">
+        <v>140</v>
+      </c>
+      <c r="E120" t="s">
+        <v>32</v>
+      </c>
+      <c r="F120" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
         <v>195</v>
       </c>
-      <c r="D120" t="s">
-        <v>196</v>
-      </c>
-      <c r="E120" t="s">
-        <v>78</v>
-      </c>
-      <c r="F120">
-        <v>5029</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>40</v>
-      </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-      <c r="C121" t="s">
-        <v>197</v>
-      </c>
-      <c r="D121" t="s">
-        <v>198</v>
+      <c r="D121">
+        <v>140</v>
       </c>
       <c r="E121" t="s">
-        <v>78</v>
-      </c>
-      <c r="F121">
-        <v>5029</v>
+        <v>32</v>
+      </c>
+      <c r="F121" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B122">
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D122" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E122" t="s">
-        <v>78</v>
-      </c>
-      <c r="F122">
-        <v>5029</v>
+        <v>32</v>
+      </c>
+      <c r="F122" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s">
+        <v>199</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123" t="s">
+        <v>32</v>
+      </c>
+      <c r="F123" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
         <v>201</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124" t="s">
+        <v>32</v>
+      </c>
+      <c r="F124" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
         <v>202</v>
       </c>
-      <c r="E123" t="s">
-        <v>78</v>
-      </c>
-      <c r="F123">
-        <v>5029</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>43</v>
-      </c>
-      <c r="B124">
-        <v>1</v>
-      </c>
-      <c r="C124" t="s">
-        <v>203</v>
-      </c>
-      <c r="D124" t="s">
-        <v>204</v>
-      </c>
-      <c r="E124" t="s">
-        <v>205</v>
-      </c>
-      <c r="F124" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>44</v>
-      </c>
-      <c r="B125">
-        <v>4</v>
-      </c>
-      <c r="C125" t="s">
-        <v>207</v>
-      </c>
-      <c r="D125" t="s">
-        <v>208</v>
+      <c r="D125">
+        <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>211</v>
-      </c>
-      <c r="D126" t="s">
-        <v>208</v>
+        <v>203</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="F126" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>40</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
       <c r="C127" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D127" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E127" t="s">
-        <v>209</v>
-      </c>
-      <c r="F127" t="s">
-        <v>210</v>
+        <v>78</v>
+      </c>
+      <c r="F127">
+        <v>5029</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>41</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
       <c r="C128" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D128" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E128" t="s">
-        <v>209</v>
-      </c>
-      <c r="F128" t="s">
-        <v>210</v>
+        <v>78</v>
+      </c>
+      <c r="F128">
+        <v>5029</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B129">
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D129" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E129" t="s">
-        <v>205</v>
-      </c>
-      <c r="F129" t="s">
-        <v>215</v>
+        <v>78</v>
+      </c>
+      <c r="F129">
+        <v>5029</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B130">
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D130" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E130" t="s">
-        <v>205</v>
-      </c>
-      <c r="F130" t="s">
-        <v>218</v>
+        <v>78</v>
+      </c>
+      <c r="F130">
+        <v>5029</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D131" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E131" t="s">
-        <v>57</v>
-      </c>
-      <c r="F131" t="s">
-        <v>220</v>
+        <v>78</v>
+      </c>
+      <c r="F131">
+        <v>5029</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D132" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E132" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F132" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
+        <v>46</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s">
+        <v>218</v>
+      </c>
+      <c r="D133" t="s">
+        <v>219</v>
+      </c>
+      <c r="E133" t="s">
+        <v>220</v>
+      </c>
+      <c r="F133" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>222</v>
+      </c>
+      <c r="D134" t="s">
+        <v>219</v>
+      </c>
+      <c r="E134" t="s">
+        <v>220</v>
+      </c>
+      <c r="F134" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>223</v>
+      </c>
+      <c r="D135" t="s">
+        <v>219</v>
+      </c>
+      <c r="E135" t="s">
+        <v>220</v>
+      </c>
+      <c r="F135" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>224</v>
+      </c>
+      <c r="D136" t="s">
+        <v>219</v>
+      </c>
+      <c r="E136" t="s">
+        <v>220</v>
+      </c>
+      <c r="F136" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>47</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>225</v>
+      </c>
+      <c r="D137" t="s">
+        <v>226</v>
+      </c>
+      <c r="E137" t="s">
+        <v>216</v>
+      </c>
+      <c r="F137" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>48</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>227</v>
+      </c>
+      <c r="D138" t="s">
+        <v>228</v>
+      </c>
+      <c r="E138" t="s">
+        <v>216</v>
+      </c>
+      <c r="F138" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
         <v>49</v>
       </c>
-      <c r="B133">
+      <c r="B139">
         <v>1</v>
       </c>
-      <c r="C133" t="s">
-        <v>225</v>
-      </c>
-      <c r="D133" t="s">
-        <v>226</v>
-      </c>
-      <c r="E133" t="s">
-        <v>223</v>
-      </c>
-      <c r="F133" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134">
+      <c r="C139" t="s">
+        <v>230</v>
+      </c>
+      <c r="D139" t="s">
+        <v>231</v>
+      </c>
+      <c r="E139" t="s">
+        <v>57</v>
+      </c>
+      <c r="F139" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
         <v>50</v>
       </c>
-      <c r="B134">
+      <c r="B140">
         <v>1</v>
       </c>
-      <c r="C134" t="s">
-        <v>227</v>
-      </c>
-      <c r="D134" t="s">
-        <v>228</v>
-      </c>
-      <c r="E134" t="s">
-        <v>205</v>
-      </c>
-      <c r="F134" t="s">
-        <v>229</v>
+      <c r="C140" t="s">
+        <v>232</v>
+      </c>
+      <c r="D140" t="s">
+        <v>233</v>
+      </c>
+      <c r="E140" t="s">
+        <v>234</v>
+      </c>
+      <c r="F140" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>51</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>236</v>
+      </c>
+      <c r="D141" t="s">
+        <v>237</v>
+      </c>
+      <c r="E141" t="s">
+        <v>234</v>
+      </c>
+      <c r="F141" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>52</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>238</v>
+      </c>
+      <c r="D142" t="s">
+        <v>239</v>
+      </c>
+      <c r="E142" t="s">
+        <v>216</v>
+      </c>
+      <c r="F142" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>